<commit_message>
Arreglos de bat y arreglos de toma de datos dolar
</commit_message>
<xml_diff>
--- a/scrap_CBT/files/Calculos.xlsx
+++ b/scrap_CBT/files/Calculos.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -15,9 +15,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -2457,7 +2456,7 @@
         <v>32448.60109358516</v>
       </c>
       <c r="G89" t="n">
-        <v>95935.4559965446</v>
+        <v>95935.45599654461</v>
       </c>
     </row>
     <row r="90">
@@ -2480,7 +2479,7 @@
         <v>37861.6278979834</v>
       </c>
       <c r="G90" t="n">
-        <v>77313.25379535164</v>
+        <v>77313.25379535166</v>
       </c>
     </row>
     <row r="91">
@@ -2503,7 +2502,7 @@
         <v>42874.52364698592</v>
       </c>
       <c r="G91" t="n">
-        <v>86746.36244998997</v>
+        <v>86746.36244998999</v>
       </c>
     </row>
     <row r="92">
@@ -2526,7 +2525,7 @@
         <v>46562.96008101164</v>
       </c>
       <c r="G92" t="n">
-        <v>93772.87719580498</v>
+        <v>93772.87719580499</v>
       </c>
     </row>
     <row r="93">

</xml_diff>

<commit_message>
Nuevo bat, para evitar fallos
</commit_message>
<xml_diff>
--- a/scrap_CBT/files/Calculos.xlsx
+++ b/scrap_CBT/files/Calculos.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -2456,7 +2456,7 @@
         <v>32448.60109358516</v>
       </c>
       <c r="G89" t="n">
-        <v>95935.4559965446</v>
+        <v>95935.45599654461</v>
       </c>
     </row>
     <row r="90">
@@ -2479,7 +2479,7 @@
         <v>37861.6278979834</v>
       </c>
       <c r="G90" t="n">
-        <v>77313.25379535164</v>
+        <v>77313.25379535166</v>
       </c>
     </row>
     <row r="91">
@@ -2502,7 +2502,7 @@
         <v>42874.52364698592</v>
       </c>
       <c r="G91" t="n">
-        <v>86746.36244998997</v>
+        <v>86746.36244998999</v>
       </c>
     </row>
     <row r="92">
@@ -2525,7 +2525,7 @@
         <v>46562.96008101164</v>
       </c>
       <c r="G92" t="n">
-        <v>93772.87719580498</v>
+        <v>93772.87719580499</v>
       </c>
     </row>
     <row r="93">

</xml_diff>

<commit_message>
Cbt Y Cba cambio en los correos
</commit_message>
<xml_diff>
--- a/scrap_CBT/files/Calculos.xlsx
+++ b/scrap_CBT/files/Calculos.xlsx
@@ -406,7 +406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2456,7 +2456,7 @@
         <v>32448.60109358516</v>
       </c>
       <c r="G89" t="n">
-        <v>95935.45599654461</v>
+        <v>95935.4559965446</v>
       </c>
     </row>
     <row r="90">
@@ -2479,7 +2479,7 @@
         <v>37861.6278979834</v>
       </c>
       <c r="G90" t="n">
-        <v>77313.25379535166</v>
+        <v>77313.25379535164</v>
       </c>
     </row>
     <row r="91">
@@ -2502,7 +2502,7 @@
         <v>42874.52364698592</v>
       </c>
       <c r="G91" t="n">
-        <v>86746.36244998999</v>
+        <v>86746.36244998997</v>
       </c>
     </row>
     <row r="92">
@@ -2525,7 +2525,7 @@
         <v>46562.96008101164</v>
       </c>
       <c r="G92" t="n">
-        <v>93772.87719580499</v>
+        <v>93772.87719580498</v>
       </c>
     </row>
     <row r="93">
@@ -2549,6 +2549,29 @@
       </c>
       <c r="G93" t="n">
         <v>106037.345858298</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B94" t="n">
+        <v>77889.58</v>
+      </c>
+      <c r="C94" t="n">
+        <v>160452.53</v>
+      </c>
+      <c r="D94" t="n">
+        <v>240678.8022</v>
+      </c>
+      <c r="E94" t="n">
+        <v>495798.3177</v>
+      </c>
+      <c r="F94" t="n">
+        <v>69779.20709593572</v>
+      </c>
+      <c r="G94" t="n">
+        <v>134645.3736769893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>